<commit_message>
Updated Occupancy and EPD for office space types
All vintages including 2007.
</commit_message>
<xml_diff>
--- a/reference/OpenStudio/MultiSpaceTypeOfficeWorksheet.xlsx
+++ b/reference/OpenStudio/MultiSpaceTypeOfficeWorksheet.xlsx
@@ -8,16 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="EPD worksheet" sheetId="2" r:id="rId2"/>
+    <sheet name="EPD worksheet Baseline" sheetId="2" r:id="rId2"/>
     <sheet name="Proposed Space Type 2004" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="129">
   <si>
     <t>Office Space Type breakdown in TSD documents.</t>
   </si>
@@ -386,6 +385,24 @@
   </si>
   <si>
     <t>OfficeClosed</t>
+  </si>
+  <si>
+    <t>AEDG</t>
+  </si>
+  <si>
+    <t>Percent of total area</t>
+  </si>
+  <si>
+    <t>AEDG EPD (W/ft^2)</t>
+  </si>
+  <si>
+    <t>AEDG Target Values</t>
+  </si>
+  <si>
+    <t>Bsaseline</t>
+  </si>
+  <si>
+    <t>AEDG equip w</t>
   </si>
 </sst>
 </file>
@@ -395,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,8 +485,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,6 +539,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -831,6 +861,41 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1141,7 +1206,7 @@
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2602,23 +2667,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="2" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="41.28515625" customWidth="1"/>
-    <col min="7" max="8" width="25.5703125" customWidth="1"/>
+    <col min="2" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" style="86" customWidth="1"/>
+    <col min="6" max="8" width="15.140625" style="86" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="10" width="41.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="86" customWidth="1"/>
+    <col min="12" max="13" width="25.5703125" customWidth="1"/>
+    <col min="14" max="14" width="25.5703125" style="86" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="N1" s="86"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>46</v>
       </c>
@@ -2629,22 +2705,40 @@
       <c r="D2" s="19">
         <v>20000</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="106" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="J2" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54"/>
-    </row>
-    <row r="3" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="53"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="101"/>
+    </row>
+    <row r="3" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43"/>
       <c r="B3" s="40"/>
       <c r="C3" s="47"/>
       <c r="D3" s="48"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="56"/>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="N3" s="56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -2657,17 +2751,33 @@
       <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="E4" s="45"/>
+      <c r="F4" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="K4" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="M4" s="59" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N4" s="59" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2681,18 +2791,38 @@
         <f>B5*C5</f>
         <v>130</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="86">
+        <f>B5*(F30/B30)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="86">
+        <v>54</v>
+      </c>
+      <c r="H5" s="86">
+        <f>F5*G5</f>
+        <v>108</v>
+      </c>
+      <c r="J5" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="43">
+      <c r="K5" s="93">
+        <f>'Proposed Space Type 2004'!$B$18</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L5" s="43">
+        <f>K5*$D$2</f>
         <v>100</v>
       </c>
-      <c r="H5" s="56">
-        <f>D5/G5</f>
+      <c r="M5" s="56">
+        <f>D5/L5</f>
         <v>1.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N5" s="56">
+        <f>H5/L5</f>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -2706,30 +2836,63 @@
         <f t="shared" ref="D6:D22" si="0">B6*C6</f>
         <v>2860</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="86">
+        <f>B6*(F31/B31)</f>
+        <v>29.223880597014926</v>
+      </c>
+      <c r="G6" s="86">
+        <v>54</v>
+      </c>
+      <c r="H6" s="86">
+        <f t="shared" ref="H6:H22" si="1">F6*G6</f>
+        <v>1578.0895522388059</v>
+      </c>
+      <c r="J6" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="43">
+      <c r="K6" s="93">
+        <f>'Proposed Space Type 2004'!$B$8</f>
+        <v>0.15</v>
+      </c>
+      <c r="L6" s="43">
+        <f t="shared" ref="L6:L23" si="2">K6*$D$2</f>
         <v>3000</v>
       </c>
-      <c r="H6" s="56">
-        <f>D6*(G6/(G6+G7))/G6</f>
+      <c r="M6" s="56">
+        <f>D6*(L6/(L6+L7))/L6</f>
         <v>0.32499999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="55" t="s">
+      <c r="N6" s="56">
+        <f>H6*(L6/(L6+L7))/L6</f>
+        <v>0.17932835820895521</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="J7" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="43">
+      <c r="K7" s="93">
+        <f>'Proposed Space Type 2004'!$B$9</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L7" s="43">
+        <f t="shared" si="2"/>
         <v>5800</v>
       </c>
-      <c r="H7" s="56">
-        <f>D6*(G7/(G6+G7))/G7</f>
+      <c r="M7" s="56">
+        <f>D6*(L7/(L6+L7))/L7</f>
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N7" s="56">
+        <f>H6*(L7/(L6+L7))/L7</f>
+        <v>0.17932835820895521</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2743,30 +2906,63 @@
         <f t="shared" si="0"/>
         <v>836</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="86">
+        <f>B8*(F32/B32)</f>
+        <v>58.776119402985074</v>
+      </c>
+      <c r="G8" s="86">
+        <v>17</v>
+      </c>
+      <c r="H8" s="86">
+        <f t="shared" si="1"/>
+        <v>999.19402985074623</v>
+      </c>
+      <c r="J8" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="43">
+      <c r="K8" s="93">
+        <f>'Proposed Space Type 2004'!$B$8</f>
+        <v>0.15</v>
+      </c>
+      <c r="L8" s="43">
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
-      <c r="H8" s="56">
-        <f>D8*(G8/(G8+G9))/G8</f>
+      <c r="M8" s="56">
+        <f>D8*(L8/(L8+L9))/L8</f>
         <v>9.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="55" t="s">
+      <c r="N8" s="56">
+        <f>H8*(L8/(L8+L9))/L8</f>
+        <v>0.11354477611940297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="J9" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="43">
+      <c r="K9" s="93">
+        <f>'Proposed Space Type 2004'!$B$9</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L9" s="43">
+        <f t="shared" si="2"/>
         <v>5800</v>
       </c>
-      <c r="H9" s="56">
-        <f>D8*(G9/(G8+G9))/G9</f>
+      <c r="M9" s="56">
+        <f>D8*(L9/(L8+L9))/L9</f>
         <v>9.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N9" s="56">
+        <f>H8*(L9/(L8+L9))/L9</f>
+        <v>0.11354477611940297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2780,18 +2976,38 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="F10" s="55" t="s">
+      <c r="F10" s="86">
+        <f>B10*(F33/B33)</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="86">
+        <v>24</v>
+      </c>
+      <c r="H10" s="86">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J10" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="43">
+      <c r="K10" s="93">
+        <f>'Proposed Space Type 2004'!$B$18</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L10" s="43">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="H10" s="56">
-        <f t="shared" ref="H10:H22" si="1">D10/G10</f>
+      <c r="M10" s="56">
+        <f>D10/L10</f>
         <v>0.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N10" s="56">
+        <f>H10/L10</f>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2805,30 +3021,63 @@
         <f t="shared" si="0"/>
         <v>3080</v>
       </c>
-      <c r="F11" s="55" t="s">
+      <c r="F11" s="86">
+        <f>B11*(F34/B34)</f>
+        <v>88</v>
+      </c>
+      <c r="G11" s="86">
+        <v>24</v>
+      </c>
+      <c r="H11" s="86">
+        <f t="shared" si="1"/>
+        <v>2112</v>
+      </c>
+      <c r="J11" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="43">
+      <c r="K11" s="93">
+        <f>'Proposed Space Type 2004'!$B$8</f>
+        <v>0.15</v>
+      </c>
+      <c r="L11" s="43">
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
-      <c r="H11" s="56">
-        <f>D11*(G11/(G11+G12))/G11</f>
+      <c r="M11" s="56">
+        <f>D11*(L11/(L11+L12))/L11</f>
         <v>0.35</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="55" t="s">
+      <c r="N11" s="56">
+        <f>H11*(L11/(L11+L12))/L11</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="J12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="43">
+      <c r="K12" s="93">
+        <f>'Proposed Space Type 2004'!$B$9</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L12" s="43">
+        <f t="shared" si="2"/>
         <v>5800</v>
       </c>
-      <c r="H12" s="56">
-        <f>D11*(G12/(G11+G12))/G12</f>
+      <c r="M12" s="56">
+        <f>D11*(L12/(L11+L12))/L12</f>
         <v>0.35</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N12" s="56">
+        <f>H11*(L12/(L11+L12))/L12</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2842,18 +3091,38 @@
         <f t="shared" si="0"/>
         <v>430</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="86">
+        <f>B13*(F35/B35)</f>
+        <v>2</v>
+      </c>
+      <c r="G13" s="86">
+        <v>180</v>
+      </c>
+      <c r="H13" s="86">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+      <c r="J13" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="43">
-        <v>400</v>
-      </c>
-      <c r="H13" s="56">
-        <f t="shared" si="1"/>
-        <v>1.075</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K13" s="93">
+        <f>'Proposed Space Type 2004'!$B$20</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L13" s="43">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="M13" s="56">
+        <f t="shared" ref="M10:N19" si="3">D13/L13</f>
+        <v>0.86</v>
+      </c>
+      <c r="N13" s="56">
+        <f>H13/L13</f>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2867,18 +3136,38 @@
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="86">
+        <f t="shared" ref="F14:F22" si="4">B14*(F36/B36)</f>
+        <v>2</v>
+      </c>
+      <c r="G14" s="86">
+        <v>500</v>
+      </c>
+      <c r="H14" s="86">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="J14" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="43">
-        <v>400</v>
-      </c>
-      <c r="H14" s="56">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K14" s="93">
+        <f>'Proposed Space Type 2004'!$B$20</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L14" s="43">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="M14" s="56">
+        <f t="shared" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N14" s="56">
+        <f>H14/L14</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2892,18 +3181,38 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="F15" s="55" t="s">
+      <c r="F15" s="86">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G15" s="86">
+        <v>17</v>
+      </c>
+      <c r="H15" s="86">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J15" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="43">
-        <v>400</v>
-      </c>
-      <c r="H15" s="56">
-        <f t="shared" si="1"/>
-        <v>0.17499999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K15" s="93">
+        <f>'Proposed Space Type 2004'!$B$20</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L15" s="43">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="M15" s="56">
+        <f t="shared" si="3"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N15" s="56">
+        <f>H15/L15</f>
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2917,18 +3226,38 @@
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="F16" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="43">
-        <v>400</v>
-      </c>
-      <c r="H16" s="56">
+      <c r="F16" s="86">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G16" s="86">
+        <v>193</v>
+      </c>
+      <c r="H16" s="86">
         <f t="shared" si="1"/>
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+      <c r="J16" s="94" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="95">
+        <f>'Proposed Space Type 2004'!$B$11</f>
+        <v>0.12</v>
+      </c>
+      <c r="L16" s="43">
+        <f t="shared" si="2"/>
+        <v>2400</v>
+      </c>
+      <c r="M16" s="56">
+        <f t="shared" si="3"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="N16" s="56">
+        <f>H16/L16</f>
+        <v>0.16083333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2942,18 +3271,38 @@
         <f t="shared" si="0"/>
         <v>152</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="86">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G17" s="86">
+        <v>65</v>
+      </c>
+      <c r="H17" s="86">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="J17" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="43">
+      <c r="K17" s="93">
+        <f>'Proposed Space Type 2004'!$B$14</f>
+        <v>0.02</v>
+      </c>
+      <c r="L17" s="43">
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
-      <c r="H17" s="56">
-        <f t="shared" si="1"/>
+      <c r="M17" s="56">
+        <f t="shared" si="3"/>
         <v>0.38</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N17" s="56">
+        <f>H17/L17</f>
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2967,18 +3316,38 @@
         <f t="shared" si="0"/>
         <v>1540</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="86">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G18" s="86">
+        <v>770</v>
+      </c>
+      <c r="H18" s="86">
+        <f t="shared" si="1"/>
+        <v>1540</v>
+      </c>
+      <c r="J18" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="43">
+      <c r="K18" s="93">
+        <f>'Proposed Space Type 2004'!$B$19</f>
+        <v>0.02</v>
+      </c>
+      <c r="L18" s="43">
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
-      <c r="H18" s="56">
-        <f t="shared" si="1"/>
+      <c r="M18" s="56">
+        <f t="shared" si="3"/>
         <v>3.85</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N18" s="56">
+        <f>H18/L18</f>
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2992,18 +3361,38 @@
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="86">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G19" s="86">
+        <v>1050</v>
+      </c>
+      <c r="H19" s="86">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="J19" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="43">
+      <c r="K19" s="93">
+        <f>'Proposed Space Type 2004'!$B$14</f>
+        <v>0.02</v>
+      </c>
+      <c r="L19" s="43">
+        <f t="shared" si="2"/>
         <v>400</v>
       </c>
-      <c r="H19" s="56">
-        <f t="shared" si="1"/>
+      <c r="M19" s="56">
+        <f>D19/L19</f>
         <v>5.25</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N19" s="56">
+        <f>H19/L19</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -3017,69 +3406,142 @@
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-      <c r="F20" s="55" t="s">
+      <c r="F20" s="86">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="G20" s="86">
+        <v>30</v>
+      </c>
+      <c r="H20" s="86">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="J20" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="43">
+      <c r="K20" s="93">
+        <f>'Proposed Space Type 2004'!$B$8</f>
+        <v>0.15</v>
+      </c>
+      <c r="L20" s="43">
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
-      <c r="H20" s="56">
-        <f>D20*(G20/(G20+G21))/G20</f>
+      <c r="M20" s="56">
+        <f>D20*(L20/(L20+L21))/L20</f>
         <v>0.10227272727272727</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="55" t="s">
+      <c r="N20" s="56">
+        <f>H20*(L20/(L20+L21))/L20</f>
+        <v>0.10227272727272727</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="86"/>
+      <c r="J21" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="43">
+      <c r="K21" s="93">
+        <f>'Proposed Space Type 2004'!$B$9</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L21" s="43">
+        <f t="shared" si="2"/>
         <v>5800</v>
       </c>
-      <c r="H21" s="56">
-        <f>D20*(G21/(G20+G21))/G21</f>
+      <c r="M21" s="56">
+        <f>D20*(L21/(L20+L21))/L21</f>
         <v>0.10227272727272727</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="N21" s="56">
+        <f>H20*(L21/(L20+L21))/L21</f>
+        <v>0.10227272727272727</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B22">
-        <v>4</v>
+      <c r="B22" s="105">
+        <v>90</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="F22" s="60" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="61">
-        <v>400</v>
-      </c>
-      <c r="H22" s="62">
+        <v>360</v>
+      </c>
+      <c r="F22" s="86">
+        <f>B22*(F43/B43)</f>
+        <v>90</v>
+      </c>
+      <c r="G22" s="86">
+        <v>4</v>
+      </c>
+      <c r="H22" s="86">
         <f t="shared" si="1"/>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+      <c r="J22" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="93">
+        <f>'Proposed Space Type 2004'!$B$8</f>
+        <v>0.15</v>
+      </c>
+      <c r="L22" s="43">
+        <f t="shared" si="2"/>
+        <v>3000</v>
+      </c>
+      <c r="M22" s="56">
+        <f>D22*(L22/(L22+L23))/L22</f>
+        <v>4.0909090909090909E-2</v>
+      </c>
+      <c r="N22" s="56">
+        <f>H22*(L22/(L22+L23))/L22</f>
+        <v>4.0909090909090909E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J23" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="104">
+        <f>'Proposed Space Type 2004'!$B$9</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L23" s="61">
+        <f t="shared" si="2"/>
+        <v>5800</v>
+      </c>
+      <c r="M23" s="62">
+        <f>D22*(L23/(L22+L23))/L23</f>
+        <v>4.0909090909090909E-2</v>
+      </c>
+      <c r="N23" s="62">
+        <f>H22*(L23/(L22+L23))/L23</f>
+        <v>4.0909090909090909E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
       <c r="D24">
         <f>SUM(D5:D22)</f>
-        <v>15084</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15428</v>
+      </c>
+      <c r="H24" s="86">
+        <f>SUM(H5:H22)</f>
+        <v>11655.283582089553</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>47</v>
       </c>
@@ -3090,20 +3552,30 @@
       <c r="D27" s="19">
         <v>54000</v>
       </c>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-    </row>
-    <row r="28" spans="1:8" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="J27" s="86"/>
+      <c r="L27" s="86"/>
+      <c r="M27" s="86"/>
+    </row>
+    <row r="28" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="43"/>
       <c r="B28" s="40"/>
       <c r="C28" s="47"/>
       <c r="D28" s="48"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="86"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
@@ -3116,11 +3588,21 @@
       <c r="D29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="45"/>
+      <c r="F29" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -3134,11 +3616,21 @@
         <f>B30*C30</f>
         <v>520</v>
       </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F30" s="86">
+        <v>8</v>
+      </c>
+      <c r="G30" s="86">
+        <v>54</v>
+      </c>
+      <c r="H30" s="86">
+        <f>F30*G30</f>
+        <v>432</v>
+      </c>
+      <c r="J30" s="86"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -3149,14 +3641,24 @@
         <v>65</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D43" si="2">B31*C31</f>
+        <f t="shared" ref="D31:D43" si="5">B31*C31</f>
         <v>8710</v>
       </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="86">
+        <v>89</v>
+      </c>
+      <c r="G31" s="86">
+        <v>54</v>
+      </c>
+      <c r="H31" s="86">
+        <f t="shared" ref="H31:H43" si="6">F31*G31</f>
+        <v>4806</v>
+      </c>
+      <c r="J31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -3167,14 +3669,24 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2546</v>
       </c>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F32" s="86">
+        <v>179</v>
+      </c>
+      <c r="G32" s="86">
+        <v>17</v>
+      </c>
+      <c r="H32" s="86">
+        <f t="shared" si="6"/>
+        <v>3043</v>
+      </c>
+      <c r="J32" s="86"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -3185,14 +3697,24 @@
         <v>35</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>280</v>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="86">
+        <v>8</v>
+      </c>
+      <c r="G33" s="86">
+        <v>24</v>
+      </c>
+      <c r="H33" s="86">
+        <f t="shared" si="6"/>
+        <v>192</v>
+      </c>
+      <c r="J33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -3203,14 +3725,24 @@
         <v>35</v>
       </c>
       <c r="D34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9380</v>
       </c>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F34" s="86">
+        <v>268</v>
+      </c>
+      <c r="G34" s="86">
+        <v>24</v>
+      </c>
+      <c r="H34" s="86">
+        <f t="shared" si="6"/>
+        <v>6432</v>
+      </c>
+      <c r="J34" s="86"/>
+      <c r="L34" s="86"/>
+      <c r="M34" s="86"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -3221,14 +3753,24 @@
         <v>215</v>
       </c>
       <c r="D35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1720</v>
       </c>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F35" s="86">
+        <v>8</v>
+      </c>
+      <c r="G35" s="86">
+        <v>180</v>
+      </c>
+      <c r="H35" s="86">
+        <f t="shared" si="6"/>
+        <v>1440</v>
+      </c>
+      <c r="J35" s="86"/>
+      <c r="L35" s="86"/>
+      <c r="M35" s="86"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -3239,14 +3781,24 @@
         <v>1100</v>
       </c>
       <c r="D36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4400</v>
       </c>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="86">
+        <v>4</v>
+      </c>
+      <c r="G36" s="86">
+        <v>500</v>
+      </c>
+      <c r="H36" s="86">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+      <c r="J36" s="86"/>
+      <c r="L36" s="86"/>
+      <c r="M36" s="86"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -3257,14 +3809,24 @@
         <v>35</v>
       </c>
       <c r="D37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>280</v>
       </c>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F37" s="86">
+        <v>8</v>
+      </c>
+      <c r="G37" s="86">
+        <v>17</v>
+      </c>
+      <c r="H37" s="86">
+        <f t="shared" si="6"/>
+        <v>136</v>
+      </c>
+      <c r="J37" s="86"/>
+      <c r="L37" s="86"/>
+      <c r="M37" s="86"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
@@ -3275,14 +3837,24 @@
         <v>350</v>
       </c>
       <c r="D38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2800</v>
       </c>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F38" s="86">
+        <v>8</v>
+      </c>
+      <c r="G38" s="86">
+        <v>193</v>
+      </c>
+      <c r="H38" s="86">
+        <f t="shared" si="6"/>
+        <v>1544</v>
+      </c>
+      <c r="J38" s="86"/>
+      <c r="L38" s="86"/>
+      <c r="M38" s="86"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -3293,14 +3865,24 @@
         <v>76</v>
       </c>
       <c r="D39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>608</v>
       </c>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F39" s="86">
+        <v>8</v>
+      </c>
+      <c r="G39" s="86">
+        <v>65</v>
+      </c>
+      <c r="H39" s="86">
+        <f t="shared" si="6"/>
+        <v>520</v>
+      </c>
+      <c r="J39" s="86"/>
+      <c r="L39" s="86"/>
+      <c r="M39" s="86"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -3311,14 +3893,24 @@
         <v>770</v>
       </c>
       <c r="D40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3080</v>
       </c>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F40" s="86">
+        <v>4</v>
+      </c>
+      <c r="G40" s="86">
+        <v>770</v>
+      </c>
+      <c r="H40" s="86">
+        <f t="shared" si="6"/>
+        <v>3080</v>
+      </c>
+      <c r="J40" s="86"/>
+      <c r="L40" s="86"/>
+      <c r="M40" s="86"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -3329,14 +3921,24 @@
         <v>1050</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4200</v>
       </c>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F41" s="86">
+        <v>4</v>
+      </c>
+      <c r="G41" s="86">
+        <v>1050</v>
+      </c>
+      <c r="H41" s="86">
+        <f t="shared" si="6"/>
+        <v>4200</v>
+      </c>
+      <c r="J41" s="86"/>
+      <c r="L41" s="86"/>
+      <c r="M41" s="86"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -3347,14 +3949,24 @@
         <v>30</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F42" s="86">
+        <v>30</v>
+      </c>
+      <c r="G42" s="86">
+        <v>30</v>
+      </c>
+      <c r="H42" s="86">
+        <f t="shared" si="6"/>
+        <v>900</v>
+      </c>
+      <c r="J42" s="86"/>
+      <c r="L42" s="86"/>
+      <c r="M42" s="86"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -3365,19 +3977,29 @@
         <v>4</v>
       </c>
       <c r="D43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1000</v>
       </c>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F43" s="86">
+        <v>250</v>
+      </c>
+      <c r="G43" s="86">
+        <v>4</v>
+      </c>
+      <c r="H43" s="86">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
+      <c r="J43" s="86"/>
+      <c r="L43" s="86"/>
+      <c r="M43" s="86"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J44" s="86"/>
+      <c r="L44" s="86"/>
+      <c r="M44" s="86"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -3385,20 +4007,45 @@
         <f>SUM(D30:D43)</f>
         <v>40424</v>
       </c>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F46" s="45"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H45" s="86">
+        <f>SUM(H30:H43)</f>
+        <v>29725</v>
+      </c>
+      <c r="J45" s="86"/>
+      <c r="L45" s="86"/>
+      <c r="M45" s="86"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J46" s="86"/>
+      <c r="L46" s="86"/>
+      <c r="M46" s="86"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J47" s="86"/>
+      <c r="L47" s="86"/>
+      <c r="M47" s="86"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J48" s="86"/>
+      <c r="L48" s="86"/>
+      <c r="M48" s="86"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
+      <c r="J49" s="86"/>
+      <c r="L49" s="86"/>
+      <c r="M49" s="86"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J50" s="86"/>
+      <c r="L50" s="86"/>
+      <c r="M50" s="86"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3407,40 +4054,43 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:R64"/>
+  <dimension ref="A2:T64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="5" width="17.28515625" style="41" customWidth="1"/>
-    <col min="6" max="11" width="17.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="41"/>
+    <col min="6" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="96" customWidth="1"/>
+    <col min="9" max="12" width="17.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="41"/>
+    <col min="18" max="18" width="9.140625" style="96"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>87</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="18">
-        <f>M22</f>
+        <f>N22</f>
         <v>173.00000000000003</v>
       </c>
       <c r="D5" s="18"/>
@@ -3449,16 +4099,18 @@
         <v>20000</v>
       </c>
       <c r="G5" s="44"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="41"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="53"/>
+      <c r="H5" s="97"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="41"/>
+      <c r="N5" s="52"/>
       <c r="O5" s="53"/>
       <c r="P5" s="53"/>
       <c r="Q5" s="53"/>
-      <c r="R5" s="54"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="107"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="54"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="41"/>
       <c r="B6" s="3"/>
       <c r="C6" s="7"/>
@@ -3466,22 +4118,24 @@
       <c r="E6" s="7"/>
       <c r="F6" s="44"/>
       <c r="G6" s="44"/>
-      <c r="H6" s="92" t="s">
+      <c r="H6" s="97"/>
+      <c r="I6" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="92"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="41"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="43"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="41"/>
+      <c r="N6" s="55"/>
       <c r="O6" s="43"/>
       <c r="P6" s="43"/>
-      <c r="Q6" s="90" t="s">
+      <c r="Q6" s="43"/>
+      <c r="R6" s="108"/>
+      <c r="S6" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="R6" s="91"/>
-    </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T6" s="91"/>
+    </row>
+    <row r="7" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
         <v>2</v>
       </c>
@@ -3501,38 +4155,44 @@
       <c r="G7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="98" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="88" t="s">
+      <c r="K7" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="L7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="M7" s="68" t="s">
+      <c r="N7" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="N7" s="69" t="s">
+      <c r="O7" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="O7" s="58" t="s">
+      <c r="P7" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="P7" s="58" t="s">
+      <c r="Q7" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="Q7" s="58" t="s">
+      <c r="R7" s="109" t="s">
+        <v>128</v>
+      </c>
+      <c r="S7" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="R7" s="59" t="s">
+      <c r="T7" s="59" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="74" t="s">
         <v>122</v>
       </c>
@@ -3552,45 +4212,53 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G8" s="89">
-        <f>0.87*0.95</f>
-        <v>0.82650000000000001</v>
-      </c>
-      <c r="H8" s="9">
+        <f>SUM('EPD worksheet Baseline'!M7,'EPD worksheet Baseline'!M9,'EPD worksheet Baseline'!M12,'EPD worksheet Baseline'!M21,'EPD worksheet Baseline'!M22)*0.95</f>
+        <v>0.86752272727272728</v>
+      </c>
+      <c r="H8" s="99">
+        <f>SUM('EPD worksheet Baseline'!N7,'EPD worksheet Baseline'!N9,'EPD worksheet Baseline'!N12,'EPD worksheet Baseline'!N21,'EPD worksheet Baseline'!N22)*0.95</f>
+        <v>0.6422522048846675</v>
+      </c>
+      <c r="I8" s="9">
         <v>20</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9">
+      <c r="J8" s="9"/>
+      <c r="K8" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K8" s="41" t="s">
+      <c r="L8" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M8" s="55">
-        <f t="shared" ref="M8:M20" si="0">(C8*B8*$F$5)/1000</f>
+      <c r="N8" s="55">
+        <f t="shared" ref="N8:N20" si="0">(C8*B8*$F$5)/1000</f>
         <v>14.25</v>
       </c>
-      <c r="N8" s="70">
-        <f>M8*D8</f>
+      <c r="O8" s="70">
+        <f>N8*D8</f>
         <v>12.112499999999999</v>
       </c>
-      <c r="O8" s="43">
+      <c r="P8" s="43">
         <f>F8*B8*$F$5</f>
         <v>3300</v>
       </c>
-      <c r="P8" s="43">
+      <c r="Q8" s="43">
         <f>G8*B8*$F$5</f>
-        <v>2479.5</v>
-      </c>
-      <c r="Q8" s="43">
-        <f>H8*C8</f>
+        <v>2602.5681818181815</v>
+      </c>
+      <c r="R8" s="108">
+        <f>H8*B8*$F$5</f>
+        <v>1926.7566146540025</v>
+      </c>
+      <c r="S8" s="43">
+        <f>I8*C8</f>
         <v>95</v>
       </c>
-      <c r="R8" s="56">
-        <f t="shared" ref="R8:R20" si="1">I8*B8*$F$5</f>
+      <c r="T8" s="56">
+        <f t="shared" ref="T8:T20" si="1">J8*B8*$F$5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="74" t="s">
         <v>119</v>
       </c>
@@ -3610,45 +4278,53 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G9" s="89">
-        <f>0.87*1.05</f>
-        <v>0.91349999999999998</v>
-      </c>
-      <c r="H9" s="9">
+        <f>SUM('EPD worksheet Baseline'!M6,'EPD worksheet Baseline'!M8,'EPD worksheet Baseline'!M11,'EPD worksheet Baseline'!M20,'EPD worksheet Baseline'!M22)*1.05</f>
+        <v>0.95884090909090902</v>
+      </c>
+      <c r="H9" s="99">
+        <f>SUM('EPD worksheet Baseline'!N6,'EPD worksheet Baseline'!N8,'EPD worksheet Baseline'!N11,'EPD worksheet Baseline'!N20,'EPD worksheet Baseline'!N22)*1.05</f>
+        <v>0.70985770013568517</v>
+      </c>
+      <c r="I9" s="9">
         <v>20</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="L9" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M9" s="55">
+      <c r="N9" s="55">
         <f t="shared" si="0"/>
         <v>30.45</v>
       </c>
-      <c r="N9" s="70">
-        <f t="shared" ref="N9:N20" si="2">M9*D9</f>
+      <c r="O9" s="70">
+        <f t="shared" ref="O9:O20" si="2">N9*D9</f>
         <v>25.8825</v>
       </c>
-      <c r="O9" s="43">
-        <f t="shared" ref="O9:O20" si="3">F9*B9*$F$5</f>
+      <c r="P9" s="43">
+        <f t="shared" ref="P9:P20" si="3">F9*B9*$F$5</f>
         <v>6380</v>
       </c>
-      <c r="P9" s="43">
-        <f t="shared" ref="P9:P20" si="4">G9*B9*$F$5</f>
-        <v>5298.2999999999993</v>
-      </c>
       <c r="Q9" s="43">
-        <f>H9*C9</f>
+        <f t="shared" ref="Q9:R20" si="4">G9*B9*$F$5</f>
+        <v>5561.2772727272722</v>
+      </c>
+      <c r="R9" s="108">
+        <f>H9*B9*$F$5</f>
+        <v>4117.1746607869736</v>
+      </c>
+      <c r="S9" s="43">
+        <f>I9*C9</f>
         <v>105</v>
       </c>
-      <c r="R9" s="56">
+      <c r="T9" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>7</v>
       </c>
@@ -3670,42 +4346,50 @@
       <c r="G10" s="9">
         <v>1</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="111">
+        <f>0.5*G10*H9/G9</f>
+        <v>0.37016448370392935</v>
+      </c>
+      <c r="I10" s="9">
         <v>20</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="L10" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M10" s="55">
+      <c r="N10" s="55">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="N10" s="70">
+      <c r="O10" s="70">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="O10" s="43">
+      <c r="P10" s="43">
         <f t="shared" si="3"/>
         <v>2080</v>
       </c>
-      <c r="P10" s="43">
+      <c r="Q10" s="43">
         <f t="shared" si="4"/>
         <v>1600</v>
       </c>
-      <c r="Q10" s="43">
-        <f>H10*C10</f>
+      <c r="R10" s="108">
+        <f>H10*B10*$F$5</f>
+        <v>592.26317392628698</v>
+      </c>
+      <c r="S10" s="43">
+        <f>I10*C10</f>
         <v>1000</v>
       </c>
-      <c r="R10" s="56">
+      <c r="T10" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>8</v>
       </c>
@@ -3725,43 +4409,52 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="9">
-        <v>0</v>
-      </c>
-      <c r="I11" s="9">
+        <f>'EPD worksheet Baseline'!M16</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H11" s="99">
+        <f>'EPD worksheet Baseline'!N16</f>
+        <v>0.16083333333333333</v>
+      </c>
+      <c r="J11" s="9">
         <v>0.05</v>
       </c>
-      <c r="J11" s="9">
+      <c r="K11" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K11" s="41" t="s">
+      <c r="L11" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M11" s="55">
+      <c r="N11" s="55">
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="N11" s="70">
+      <c r="O11" s="70">
         <f t="shared" si="2"/>
         <v>2.04</v>
       </c>
-      <c r="O11" s="43">
+      <c r="P11" s="43">
         <f t="shared" si="3"/>
         <v>1200</v>
       </c>
-      <c r="P11" s="43">
+      <c r="Q11" s="43">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="43">
-        <f>I11*C11</f>
+        <v>700.00000000000011</v>
+      </c>
+      <c r="R11" s="108">
+        <f>H11*B11*$F$5</f>
+        <v>385.99999999999994</v>
+      </c>
+      <c r="S11" s="43">
+        <f>J11*C11</f>
         <v>0.05</v>
       </c>
-      <c r="R11" s="56">
+      <c r="T11" s="56">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>9</v>
       </c>
@@ -3777,42 +4470,49 @@
       <c r="G12" s="9">
         <v>0</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9">
+      <c r="H12" s="99">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9">
         <v>0.05</v>
       </c>
-      <c r="J12" s="9">
+      <c r="K12" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K12" s="41" t="s">
+      <c r="L12" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M12" s="55">
+      <c r="N12" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N12" s="70">
+      <c r="O12" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O12" s="43">
+      <c r="P12" s="43">
         <f t="shared" si="3"/>
         <v>2240.0000000000005</v>
       </c>
-      <c r="P12" s="43">
+      <c r="Q12" s="43">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="43">
-        <f t="shared" ref="Q12:Q20" si="5">H12*C12</f>
+      <c r="R12" s="108">
+        <f>H12*B12*$F$5</f>
         <v>0</v>
       </c>
-      <c r="R12" s="56">
+      <c r="S12" s="43">
+        <f t="shared" ref="S12:S20" si="5">I12*C12</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="56">
         <f t="shared" si="1"/>
         <v>140.00000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>95</v>
       </c>
@@ -3834,42 +4534,49 @@
       <c r="G13" s="9">
         <v>0.27</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="72">
+      <c r="H13" s="99">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="72">
         <v>0.96</v>
       </c>
-      <c r="J13" s="9">
+      <c r="K13" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K13" s="41" t="s">
+      <c r="L13" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M13" s="55">
+      <c r="N13" s="55">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="N13" s="70">
+      <c r="O13" s="70">
         <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
-      <c r="O13" s="43">
+      <c r="P13" s="43">
         <f t="shared" si="3"/>
         <v>640</v>
       </c>
-      <c r="P13" s="43">
+      <c r="Q13" s="43">
         <f t="shared" si="4"/>
         <v>216</v>
       </c>
-      <c r="Q13" s="43">
+      <c r="R13" s="108">
+        <f>H13*B13*$F$5</f>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="S13" s="43">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R13" s="56">
+      <c r="T13" s="56">
         <f t="shared" si="1"/>
         <v>767.99999999999989</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
         <v>100</v>
       </c>
@@ -3889,44 +4596,53 @@
         <v>1.2</v>
       </c>
       <c r="G14" s="9">
-        <v>7.42</v>
-      </c>
-      <c r="H14" s="9">
+        <f>SUM('EPD worksheet Baseline'!M17,'EPD worksheet Baseline'!M19)</f>
+        <v>5.63</v>
+      </c>
+      <c r="H14" s="99">
+        <f>SUM('EPD worksheet Baseline'!N17,'EPD worksheet Baseline'!N19)*0.8</f>
+        <v>4.46</v>
+      </c>
+      <c r="I14" s="9">
         <v>15</v>
       </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="9">
+      <c r="J14" s="10"/>
+      <c r="K14" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K14" s="41" t="s">
+      <c r="L14" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M14" s="55">
+      <c r="N14" s="55">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="N14" s="70">
+      <c r="O14" s="70">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="O14" s="43">
+      <c r="P14" s="43">
         <f t="shared" si="3"/>
         <v>480</v>
       </c>
-      <c r="P14" s="43">
+      <c r="Q14" s="43">
         <f t="shared" si="4"/>
-        <v>2968</v>
-      </c>
-      <c r="Q14" s="43">
+        <v>2252</v>
+      </c>
+      <c r="R14" s="108">
+        <f>H14*B14*$F$5</f>
+        <v>1784</v>
+      </c>
+      <c r="S14" s="43">
         <f t="shared" si="5"/>
         <v>750</v>
       </c>
-      <c r="R14" s="56">
+      <c r="T14" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
         <v>38</v>
       </c>
@@ -3942,42 +4658,49 @@
       <c r="G15" s="9">
         <v>0.27</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="99">
+        <v>0.27</v>
+      </c>
+      <c r="I15" s="9">
         <v>20</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="9">
+      <c r="J15" s="10"/>
+      <c r="K15" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K15" s="41" t="s">
+      <c r="L15" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M15" s="55">
+      <c r="N15" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N15" s="70">
+      <c r="O15" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O15" s="43">
+      <c r="P15" s="43">
         <f t="shared" si="3"/>
         <v>600</v>
       </c>
-      <c r="P15" s="43">
+      <c r="Q15" s="43">
         <f t="shared" si="4"/>
         <v>108</v>
       </c>
-      <c r="Q15" s="43">
+      <c r="R15" s="108">
+        <f>H15*B15*$F$5</f>
+        <v>108</v>
+      </c>
+      <c r="S15" s="43">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R15" s="56">
+      <c r="T15" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
         <v>69</v>
       </c>
@@ -3993,42 +4716,49 @@
       <c r="G16" s="9">
         <v>0</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9">
+      <c r="H16" s="99">
+        <v>0</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9">
         <v>0.05</v>
       </c>
-      <c r="J16" s="9">
+      <c r="K16" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K16" s="41" t="s">
+      <c r="L16" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M16" s="55">
+      <c r="N16" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N16" s="70">
+      <c r="O16" s="70">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O16" s="43">
+      <c r="P16" s="43">
         <f t="shared" si="3"/>
         <v>360</v>
       </c>
-      <c r="P16" s="43">
+      <c r="Q16" s="43">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="43">
+      <c r="R16" s="108">
+        <f>H16*B16*$F$5</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="43">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R16" s="56">
+      <c r="T16" s="56">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="s">
         <v>13</v>
       </c>
@@ -4048,44 +4778,51 @@
         <v>1.3</v>
       </c>
       <c r="G17" s="9">
+        <v>0.27</v>
+      </c>
+      <c r="H17" s="111">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H17" s="9">
+      <c r="I17" s="9">
         <v>15</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9">
+      <c r="J17" s="9"/>
+      <c r="K17" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K17" s="41" t="s">
+      <c r="L17" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M17" s="55">
+      <c r="N17" s="55">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="N17" s="70">
+      <c r="O17" s="70">
         <f t="shared" si="2"/>
         <v>4.8000000000000007</v>
       </c>
-      <c r="O17" s="43">
+      <c r="P17" s="43">
         <f t="shared" si="3"/>
         <v>1560</v>
       </c>
-      <c r="P17" s="43">
+      <c r="Q17" s="43">
         <f t="shared" si="4"/>
+        <v>324</v>
+      </c>
+      <c r="R17" s="108">
+        <f>H17*B17*$F$5</f>
         <v>84.000000000000014</v>
       </c>
-      <c r="Q17" s="43">
+      <c r="S17" s="43">
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
-      <c r="R17" s="56">
+      <c r="T17" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>99</v>
       </c>
@@ -4105,44 +4842,53 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G18" s="9">
+        <f>SUM('EPD worksheet Baseline'!M5,'EPD worksheet Baseline'!M10)</f>
         <v>2</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9">
+      <c r="H18" s="99">
+        <f>SUM('EPD worksheet Baseline'!N5,'EPD worksheet Baseline'!N10)</f>
+        <v>1.56</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9">
         <v>0.05</v>
       </c>
-      <c r="J18" s="9">
+      <c r="K18" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K18" s="41" t="s">
+      <c r="L18" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M18" s="55">
+      <c r="N18" s="55">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="N18" s="70">
+      <c r="O18" s="70">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="O18" s="43">
+      <c r="P18" s="43">
         <f t="shared" si="3"/>
         <v>110.00000000000001</v>
       </c>
-      <c r="P18" s="43">
+      <c r="Q18" s="43">
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="Q18" s="43">
+      <c r="R18" s="108">
+        <f>H18*B18*$F$5</f>
+        <v>156</v>
+      </c>
+      <c r="S18" s="43">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R18" s="56">
+      <c r="T18" s="56">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>67</v>
       </c>
@@ -4162,44 +4908,53 @@
         <v>0.5</v>
       </c>
       <c r="G19" s="9">
-        <v>5.25</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9">
+        <f>'EPD worksheet Baseline'!M18</f>
+        <v>3.85</v>
+      </c>
+      <c r="H19" s="99">
+        <f>'EPD worksheet Baseline'!N18</f>
+        <v>3.85</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9">
         <v>0.05</v>
       </c>
-      <c r="J19" s="9">
+      <c r="K19" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K19" s="41" t="s">
+      <c r="L19" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M19" s="55">
+      <c r="N19" s="55">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="N19" s="70">
+      <c r="O19" s="70">
         <f t="shared" si="2"/>
         <v>0.16000000000000003</v>
       </c>
-      <c r="O19" s="43">
+      <c r="P19" s="43">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="P19" s="43">
+      <c r="Q19" s="43">
         <f t="shared" si="4"/>
-        <v>2100</v>
-      </c>
-      <c r="Q19" s="43">
+        <v>1540</v>
+      </c>
+      <c r="R19" s="108">
+        <f>H19*B19*$F$5</f>
+        <v>1540</v>
+      </c>
+      <c r="S19" s="43">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R19" s="56">
+      <c r="T19" s="56">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>98</v>
       </c>
@@ -4219,44 +4974,53 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G20" s="9">
-        <v>6.75</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9">
+        <f>SUM('EPD worksheet Baseline'!M13,'EPD worksheet Baseline'!M14,'EPD worksheet Baseline'!M15)</f>
+        <v>5.4</v>
+      </c>
+      <c r="H20" s="99">
+        <f>SUM('EPD worksheet Baseline'!N13,'EPD worksheet Baseline'!N14,'EPD worksheet Baseline'!N15)</f>
+        <v>2.7879999999999998</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9">
         <v>0.05</v>
       </c>
-      <c r="J20" s="9">
+      <c r="K20" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K20" s="41" t="s">
+      <c r="L20" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M20" s="55">
+      <c r="N20" s="55">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="N20" s="70">
+      <c r="O20" s="70">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O20" s="43">
+      <c r="P20" s="43">
         <f t="shared" si="3"/>
         <v>550.00000000000011</v>
       </c>
-      <c r="P20" s="43">
+      <c r="Q20" s="43">
         <f t="shared" si="4"/>
-        <v>3375</v>
-      </c>
-      <c r="Q20" s="43">
+        <v>2700</v>
+      </c>
+      <c r="R20" s="108">
+        <f>H20*B20*$F$5</f>
+        <v>1394</v>
+      </c>
+      <c r="S20" s="43">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R20" s="56">
+      <c r="T20" s="56">
         <f t="shared" si="1"/>
         <v>25.000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
       <c r="B21" s="49"/>
       <c r="C21" s="9"/>
@@ -4264,18 +5028,20 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="10"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="41"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="70"/>
-      <c r="O21" s="43"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="41"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="70"/>
       <c r="P21" s="43"/>
       <c r="Q21" s="43"/>
-      <c r="R21" s="56"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R21" s="108"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="56"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
         <v>14</v>
       </c>
@@ -4284,77 +5050,87 @@
         <v>1</v>
       </c>
       <c r="C22" s="51">
-        <f>(M22/F5)*1000</f>
+        <f>(N22/F5)*1000</f>
         <v>8.6500000000000021</v>
       </c>
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
       <c r="F22" s="9">
-        <f>O22/$F$5</f>
+        <f>P22/$F$5</f>
         <v>0.98499999999999999</v>
       </c>
       <c r="G22" s="9">
-        <f>P22/$F$5</f>
-        <v>0.92143999999999993</v>
-      </c>
-      <c r="H22" s="9">
-        <f>Q22/C5</f>
+        <f>Q22/$F$5</f>
+        <v>0.89019227272727253</v>
+      </c>
+      <c r="H22" s="99">
+        <f>R22/$F$5</f>
+        <v>0.60720972246836313</v>
+      </c>
+      <c r="I22" s="9">
+        <f>S22/C5</f>
         <v>12.139017341040461</v>
       </c>
-      <c r="I22" s="9">
-        <f>R22/F5</f>
+      <c r="J22" s="9">
+        <f>T22/F5</f>
         <v>5.5399999999999998E-2</v>
       </c>
-      <c r="J22" s="9">
+      <c r="K22" s="9">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="K22" s="41" t="s">
+      <c r="L22" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="M22" s="60">
-        <f t="shared" ref="M22:R22" si="6">SUM(M8:M20)</f>
+      <c r="N22" s="60">
+        <f t="shared" ref="N22:T22" si="6">SUM(N8:N20)</f>
         <v>173.00000000000003</v>
       </c>
-      <c r="N22" s="71">
+      <c r="O22" s="71">
         <f t="shared" si="6"/>
         <v>90.39500000000001</v>
       </c>
-      <c r="O22" s="61">
+      <c r="P22" s="61">
         <f t="shared" si="6"/>
         <v>19700</v>
       </c>
-      <c r="P22" s="61">
-        <f t="shared" si="6"/>
-        <v>18428.8</v>
-      </c>
       <c r="Q22" s="61">
         <f t="shared" si="6"/>
+        <v>17803.845454545452</v>
+      </c>
+      <c r="R22" s="110">
+        <f t="shared" ref="R22" si="7">SUM(R8:R20)</f>
+        <v>12144.194449367264</v>
+      </c>
+      <c r="S22" s="61">
+        <f t="shared" si="6"/>
         <v>2100.0500000000002</v>
       </c>
-      <c r="R22" s="62">
+      <c r="T22" s="62">
         <f t="shared" si="6"/>
         <v>1108</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="49"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="H23" s="99"/>
       <c r="I23" s="9"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="2"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="70"/>
-      <c r="O23" s="43"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="2"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="70"/>
       <c r="P23" s="43"/>
       <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="108"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>56</v>
       </c>
@@ -4372,28 +5148,29 @@
       <c r="G24" s="32">
         <v>1</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="100"/>
+      <c r="I24" s="32">
         <v>21.86</v>
       </c>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33">
+      <c r="J24" s="33"/>
+      <c r="K24" s="33">
         <v>5.94487E-2</v>
       </c>
-      <c r="K24" s="34">
+      <c r="L24" s="34">
         <v>0.25</v>
       </c>
-      <c r="N24" s="23">
-        <f>N22*1000/F5</f>
+      <c r="O24" s="23">
+        <f>O22*1000/F5</f>
         <v>4.519750000000001</v>
       </c>
-      <c r="O24" s="41" t="s">
+      <c r="P24" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="P24" s="41"/>
       <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-    </row>
-    <row r="25" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S24" s="41"/>
+      <c r="T24" s="41"/>
+    </row>
+    <row r="25" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>57</v>
       </c>
@@ -4411,25 +5188,27 @@
       <c r="G25" s="32">
         <v>1</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="100"/>
+      <c r="I25" s="32">
         <v>26.48</v>
       </c>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33">
+      <c r="J25" s="33"/>
+      <c r="K25" s="33">
         <v>5.94487E-2</v>
       </c>
-      <c r="K25" s="34">
+      <c r="L25" s="34">
         <v>0.25</v>
       </c>
-      <c r="N25" s="41">
+      <c r="O25" s="41">
         <f>C24*0.95</f>
         <v>4.75</v>
       </c>
-      <c r="O25" s="41" t="s">
+      <c r="P25" s="41" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R25" s="96"/>
+    </row>
+    <row r="26" spans="1:20" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>58</v>
       </c>
@@ -4447,42 +5226,44 @@
       <c r="G26" s="32">
         <v>1</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="100"/>
+      <c r="I26" s="32">
         <v>26.48</v>
       </c>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33">
+      <c r="J26" s="33"/>
+      <c r="K26" s="33">
         <v>5.94487E-2</v>
       </c>
-      <c r="K26" s="34">
+      <c r="L26" s="34">
         <v>0.25</v>
       </c>
-      <c r="N26" s="41">
+      <c r="O26" s="41">
         <f>0.95* 88*1000/20000</f>
         <v>4.18</v>
       </c>
-      <c r="O26" s="41" t="s">
+      <c r="P26" s="41" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R26" s="96"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
       <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
       <c r="I28" s="41"/>
       <c r="J28" s="41"/>
       <c r="K28" s="41"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L28" s="41"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="63"/>
       <c r="B29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="45"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B31" s="45" t="s">
         <v>81</v>
       </c>
@@ -4494,7 +5275,7 @@
       </c>
       <c r="E31" s="45"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>82</v>
       </c>
@@ -4506,7 +5287,7 @@
       </c>
       <c r="E32" s="44"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -4517,9 +5298,9 @@
         <v>88</v>
       </c>
       <c r="E33" s="44"/>
-      <c r="N33"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>4</v>
       </c>
@@ -4530,23 +5311,23 @@
         <v>88</v>
       </c>
       <c r="E34" s="44"/>
-      <c r="N34"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="73"/>
       <c r="B37" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="N37"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B39" s="41" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="41"/>
-      <c r="N39"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="52"/>
       <c r="C40" s="66" t="s">
         <v>89</v>
@@ -4557,39 +5338,39 @@
       <c r="E40" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="N40"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="55" t="s">
         <v>104</v>
       </c>
       <c r="C41" s="76">
-        <f>Q22</f>
+        <f>S22</f>
         <v>2100.0500000000002</v>
       </c>
       <c r="D41" s="76">
-        <f>H24*C24*F5/1000</f>
+        <f>I24*C24*F5/1000</f>
         <v>2186</v>
       </c>
       <c r="E41" s="77">
-        <f>H25*C25*F5/1000</f>
+        <f>I25*C25*F5/1000</f>
         <v>2648</v>
       </c>
-      <c r="N41"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B42" s="55" t="s">
         <v>105</v>
       </c>
       <c r="C42" s="76">
-        <f>R22</f>
+        <f>T22</f>
         <v>1108</v>
       </c>
       <c r="D42" s="76"/>
       <c r="E42" s="77"/>
-      <c r="N42"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B43" s="60" t="s">
         <v>74</v>
       </c>
@@ -4605,79 +5386,99 @@
         <f>SUM(E41:E42)</f>
         <v>2648</v>
       </c>
-      <c r="N43"/>
-    </row>
-    <row r="44" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O43"/>
+    </row>
+    <row r="44" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
       <c r="D44" s="43"/>
       <c r="E44" s="43"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H44" s="96"/>
+      <c r="R44" s="96"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="74"/>
       <c r="B46" t="s">
         <v>102</v>
       </c>
       <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
       <c r="I46" s="41"/>
       <c r="J46" s="41"/>
       <c r="K46" s="41"/>
-      <c r="N46"/>
-    </row>
-    <row r="47" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L46" s="41"/>
+      <c r="O46"/>
+    </row>
+    <row r="47" spans="1:18" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="96"/>
+      <c r="R47" s="96"/>
+    </row>
+    <row r="48" spans="1:18" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="86" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="96"/>
+      <c r="R48" s="96"/>
+    </row>
+    <row r="49" spans="1:18" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="86" t="s">
         <v>120</v>
       </c>
       <c r="D49" s="86" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H49" s="96"/>
+      <c r="R49" s="96"/>
+    </row>
+    <row r="50" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="96"/>
+      <c r="R50" s="96"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="75"/>
       <c r="B52" t="s">
         <v>103</v>
       </c>
       <c r="D52"/>
       <c r="E52"/>
-      <c r="N52"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="87"/>
       <c r="B55" t="s">
         <v>110</v>
       </c>
       <c r="F55" s="81"/>
     </row>
-    <row r="56" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="86" t="s">
         <v>116</v>
       </c>
       <c r="F56" s="81"/>
-    </row>
-    <row r="57" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="96"/>
+      <c r="R56" s="96"/>
+    </row>
+    <row r="57" spans="1:18" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F57" s="81"/>
-    </row>
-    <row r="58" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="96"/>
+      <c r="R57" s="96"/>
+    </row>
+    <row r="58" spans="1:18" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="86" t="s">
         <v>117</v>
       </c>
       <c r="F58" s="81"/>
-    </row>
-    <row r="59" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="96"/>
+      <c r="R58" s="96"/>
+    </row>
+    <row r="59" spans="1:18" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="81" t="s">
         <v>115</v>
       </c>
       <c r="F59" s="81"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H59" s="96"/>
+      <c r="R59" s="96"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B60" s="44" t="s">
         <v>111</v>
       </c>
@@ -4686,7 +5487,7 @@
       </c>
       <c r="D60" s="83"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B61" s="44" t="s">
         <v>112</v>
       </c>
@@ -4694,7 +5495,7 @@
         <v>0.22320000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B62" s="44">
         <v>2004</v>
       </c>
@@ -4702,7 +5503,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B63" s="44" t="s">
         <v>113</v>
       </c>
@@ -4710,7 +5511,7 @@
         <v>5.9499999999999997E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B64" s="44" t="s">
         <v>114</v>
       </c>
@@ -4720,8 +5521,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>